<commit_message>
feat: Change Scriptable Object to Xlsx
한글 문자열을 위해 vbs 파일에서 save 옵션을 6에서 62로 수정(ANSI -> UTF8)
</commit_message>
<xml_diff>
--- a/DataBase/Data/Item.xlsx
+++ b/DataBase/Data/Item.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Seoultech\Github\Unity\Project_G\DataBase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A262BB93-F49A-4D27-A7D3-4BD916E9B99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BBE253-0723-4D84-97F6-4FDD6BF64287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,23 +35,180 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ironIngot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>coin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>apple</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>icon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tooltip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>HealAmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Damage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecoveryAmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>안테나</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전파수신장치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>CPU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중앙처리장치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마더보드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴퓨터메인부품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>motherboard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transistor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트랜지스터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연산보조장치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>폭발건틀릿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닿으면 폭발한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gauntlet_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레이저건</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무서운 레이저를 쏜다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LaserGun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나노블레이드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분자단위로 베어내는 무기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NanoBlade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>녹슨 파이프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weapon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>antena</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>철괴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ingots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력포션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력을 회복한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배가 고플 때 먹으면 좋을 것 같다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다양한 걸 만들 수 있을 것 같다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -377,50 +534,437 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>1001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2001</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2002</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2003</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2004</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5">
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3001</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>4001</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>4101</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add Weapon Effect
</commit_message>
<xml_diff>
--- a/DataBase/Data/Item.xlsx
+++ b/DataBase/Data/Item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Seoultech\Github\Unity\Project_G\DataBase\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5AB996-4239-43B6-8952-3AE9F562EB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4575B04-4211-43F8-8BA3-23A050D8BB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2025" yWindow="10035" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,10 +140,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Gauntlet_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>레이저건</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -152,10 +148,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LaserGun</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>나노블레이드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -233,6 +225,14 @@
   </si>
   <si>
     <t>gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gauntlet_icon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LaserGun_icon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -561,7 +561,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -644,13 +644,13 @@
         <v>1001</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -682,7 +682,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -708,13 +708,13 @@
         <v>1003</v>
       </c>
       <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -740,13 +740,13 @@
         <v>1004</v>
       </c>
       <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
         <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -778,7 +778,7 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -900,13 +900,13 @@
         <v>3001</v>
       </c>
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -935,7 +935,7 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
         <v>2</v>
@@ -964,13 +964,13 @@
         <v>4101</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E13">
         <v>20</v>
@@ -996,13 +996,13 @@
         <v>4102</v>
       </c>
       <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" t="s">
-        <v>48</v>
       </c>
       <c r="E14">
         <v>20</v>
@@ -1028,13 +1028,13 @@
         <v>4103</v>
       </c>
       <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
         <v>50</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>52</v>
       </c>
       <c r="E15">
         <v>20</v>

</xml_diff>